<commit_message>
Ikelta mano kiek sugaista laiko.
</commit_message>
<xml_diff>
--- a/ZilvinoAtaskaitosDalis/ZilvinoSugaistaLaiko.xlsx
+++ b/ZilvinoAtaskaitosDalis/ZilvinoSugaistaLaiko.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zilvinas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zilvinas\Desktop\KinoPasaulis\ZilvinoAtaskaitosDalis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Veikla</t>
   </si>
@@ -32,21 +32,6 @@
     <t>Laikas</t>
   </si>
   <si>
-    <t>Analizė</t>
-  </si>
-  <si>
-    <t>Projektavimas</t>
-  </si>
-  <si>
-    <t>Realizavimas – kurti filmą realizavimas</t>
-  </si>
-  <si>
-    <t>Realizavimas – redaguoti filmą realizavimas</t>
-  </si>
-  <si>
-    <t>Realizavimas – šalinti filmą realizavimas</t>
-  </si>
-  <si>
     <t>Realizavimas – kurti darbo skelbimą realizavimas</t>
   </si>
   <si>
@@ -71,10 +56,46 @@
     <t>Realizavimas – kino studijos filmų ataskaitos puslapio realizavimas</t>
   </si>
   <si>
-    <t>Testavimas</t>
-  </si>
-  <si>
     <t>Iš viso:</t>
+  </si>
+  <si>
+    <t>Realizavimas - filmo informacijos puslapio realizavimas</t>
+  </si>
+  <si>
+    <t>Projektavimas - kino studijos posistemės panaudos atvejų sekų diagramos</t>
+  </si>
+  <si>
+    <t>Technologijų analizė - "Redux"</t>
+  </si>
+  <si>
+    <t>Technologijų analizė - "ASP.NET Core"</t>
+  </si>
+  <si>
+    <t>Technologijų analizė - "Entity Framework Core"</t>
+  </si>
+  <si>
+    <t>Kino studijos posistemės testavimas ir klaidų taisymas</t>
+  </si>
+  <si>
+    <t>Kino studijos vartotojo vadovo sudarymas</t>
+  </si>
+  <si>
+    <t>Ataskaita</t>
+  </si>
+  <si>
+    <t>Funkciniai reikalavimai kino studijos posistemei - klasių diagrama, panaudos atvejų diagrama</t>
+  </si>
+  <si>
+    <t>Technologijų analizė - "React" ir "React-Bootstrap"</t>
+  </si>
+  <si>
+    <t>Realizavimas – PA "Kurti filmą"</t>
+  </si>
+  <si>
+    <t>Realizavimas – PA "Redaguoti filmą"</t>
+  </si>
+  <si>
+    <t>Realizavimas –PA "Šalinti filmą"</t>
   </si>
 </sst>
 </file>
@@ -451,22 +472,22 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A26" sqref="A26:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="84.42578125" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2">
         <f xml:space="preserve"> SUM(B3:B163)</f>
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,172 +499,180 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1">
         <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>3</v>
+      <c r="B12" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>

</xml_diff>